<commit_message>
made changes and latest running
</commit_message>
<xml_diff>
--- a/src/outputs/compliance_rules.xlsx
+++ b/src/outputs/compliance_rules.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,98 +443,84 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1. Rule 1: The system must comply with data privacy regulations while handling Aadhaar and PAN card details for OCR and verification.</t>
+          <t>NFR Compliance Rules:</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2. Rule 2: The system must comply with credit bureau (CIBIL) regulations while fetching credit score.</t>
+          <t>1. The system must be compliant with data privacy and protection laws, ensuring that all customer data, including Aadhaar and PAN details, are securely stored and processed.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3. Rule 3: The AI-based eligibility and risk assessment module must be transparent and explainable, adhering to AI ethics and regulations.</t>
+          <t>2. The system must comply with the regulations of the credit bureau (CIBIL) when fetching credit scores.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4. Rule 4: The system must comply with KYC regulations during real-time document verification.</t>
+          <t>3. The AI-based eligibility and risk assessment module must comply with fair lending laws and not discriminate based on prohibited factors.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5. Rule 5: The OTP-based authentication for loan sanction and e-agreement signing must comply with two-factor authentication regulations.</t>
+          <t>4. The KYC document verification process must comply with the guidelines laid down by the Reserve Bank of India (RBI) and other regulatory bodies.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>6. Rule 6: The system must comply with banking regulations during integration with core banking for disbursement.</t>
+          <t>5. The OTP-based authentication for loan sanction and e-agreement signing must comply with the standards set by the regulatory bodies for digital signatures.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>7. Rule 7: The e-sign integration using DigiLocker + Aadhaar eKYC must comply with digital signature regulations.</t>
+          <t>6. The system must ensure compliance with core banking integration standards and protocols.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>8. Rule 8: The system must comply with language regulations, supporting both English and Hindi.</t>
+          <t>7. The system must comply with the language requirements, supporting both English and Hindi.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>9. Rule 9: The system must comply with banking regulations, disbursing loans only through verified bank accounts.</t>
+          <t>8. The system must ensure compliance with the regulations for loan disbursement through verified bank accounts only.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10. Rule 10: The system must be prepared to adapt to compliance changes due to upcoming RBI guidelines.</t>
+          <t>9. The system must be prepared to adapt to compliance changes due to upcoming RBI guidelines.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>11. Rule 11: The system must ensure data security and privacy, especially with the integration of external APIs such as the credit bureau and DigiLocker.</t>
+          <t>10. The system must ensure compliance with the timeline as per the project schedule.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>12. Rule 12: The system must comply with accessibility regulations, ensuring the web app is responsive and user-friendly.</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>13. Rule 13: The system must comply with data retention and deletion policies, particularly with sensitive customer data such as Aadhaar, PAN, and bank account details.</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>14. Rule 14: The system must comply with audit trail requirements, maintaining a record of all actions performed within the system.</t>
+          <t>11. The system must meet the success metrics in compliance with the business objectives, including reducing TAT, reducing manual data entry, and increasing accuracy in eligibility checks.</t>
         </is>
       </c>
     </row>

</xml_diff>